<commit_message>
ajout du divider et des signed
</commit_message>
<xml_diff>
--- a/Table d'instruction.xlsx
+++ b/Table d'instruction.xlsx
@@ -5,18 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Etienne Drouin\Documents\Universite\2020_Hiver\GIF-4201\Projet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Etienne Drouin\Documents\Universite\2020_Hiver\GIF-4201\Projet\GIF-4201-ALU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5732D99-0BC8-4D14-A640-572D9F227195}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB689ABB-B5A3-4341-8B71-B1417E22A756}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{293095C2-1D30-4A82-B8A2-EC23183E2832}"/>
+    <workbookView xWindow="5160" yWindow="3864" windowWidth="13824" windowHeight="7176" xr2:uid="{293095C2-1D30-4A82-B8A2-EC23183E2832}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -534,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2B6103A-6221-4046-B17A-F541B5FA2722}">
   <dimension ref="B3:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>